<commit_message>
Antibody updates: * field meta information updates * model properties for target protein information * target protein link fields
* change date_type 'otherreagent' to 'other_reagent'
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Area" vbProcedure="false">{#NAME?}</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Area" vbProcedure="false">{#name?}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Sheet_Title" vbProcedure="false">"Sheet1"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>AR_Name</t>
   </si>
@@ -244,9 +244,6 @@
   </si>
   <si>
     <t>AB_2336066</t>
-  </si>
-  <si>
-    <t>HMSL200005</t>
   </si>
   <si>
     <t>g33-ligand</t>
@@ -411,7 +408,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -668,47 +665,45 @@
       <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>60</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
set "max_size" for SpooledTemporaryFile, update test data: * set max_size to 100kb for SpooledTemporaryFile used with dataset downloads * resolves #400 * update test data files so current datasets can be loaded in the testing environment * rename test data files for consistency
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4815" windowWidth="21630" windowHeight="4875" tabRatio="449"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21630" windowHeight="4530" tabRatio="449"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">{#NAME?}</definedName>
     <definedName name="Excel_BuiltIn_Sheet_Title" localSheetId="0">"Sheet1"</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -152,18 +152,6 @@
     <t>D68F8</t>
   </si>
   <si>
-    <t>AB_10694639</t>
-  </si>
-  <si>
-    <t>AB_10892861</t>
-  </si>
-  <si>
-    <t>AB_916160</t>
-  </si>
-  <si>
-    <t>AB_10695861</t>
-  </si>
-  <si>
     <t>Homo sapiens</t>
   </si>
   <si>
@@ -252,9 +240,6 @@
   </si>
   <si>
     <t>HMSL80007</t>
-  </si>
-  <si>
-    <t>AB_10563748</t>
   </si>
   <si>
     <t>Oryctolagus cuniculus</t>
@@ -277,19 +262,40 @@
   <si>
     <t xml:space="preserve">gamma immunoglobin heavy and light chains
 </t>
+  </si>
+  <si>
+    <t>AB_10892861</t>
+  </si>
+  <si>
+    <t>AB_916160</t>
+  </si>
+  <si>
+    <t>AB_10695861</t>
+  </si>
+  <si>
+    <t>AB_10563748</t>
+  </si>
+  <si>
+    <t>AB_10694639</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -302,6 +308,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -329,17 +336,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +660,9 @@
     <col min="1" max="1" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="7"/>
     <col min="4" max="4" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="7"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="6" max="6" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7"/>
     <col min="8" max="8" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="20" width="9.140625" style="7"/>
     <col min="21" max="21" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -675,7 +685,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -743,7 +753,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>29</v>
@@ -754,58 +764,58 @@
       <c r="E2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>44</v>
+      <c r="F2" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="U2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="V2" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>30</v>
@@ -816,55 +826,55 @@
       <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>45</v>
+      <c r="F3" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>31</v>
@@ -876,54 +886,54 @@
         <v>40</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="M4" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="U4" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>32</v>
@@ -935,54 +945,54 @@
         <v>41</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="V5" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>33</v>
@@ -993,55 +1003,55 @@
       <c r="E6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>46</v>
+      <c r="F6" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>34</v>
@@ -1052,103 +1062,103 @@
       <c r="E7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>47</v>
+      <c r="F7" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="U7" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify antibody.target_protein values to many-to-many relationship
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,11 +15,16 @@
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Sheet_Title" vbProcedure="false">"Sheet1"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>Changed from: AR_Center_Specific_ID</t>
   </si>
@@ -27,6 +32,9 @@
     <t>not used at this time (but still required in this sheet)</t>
   </si>
   <si>
+    <t>Changed from: target_protein_lincs_id</t>
+  </si>
+  <si>
     <t>AR_Name</t>
   </si>
   <si>
@@ -51,7 +59,7 @@
     <t>AR_Antibody_Type</t>
   </si>
   <si>
-    <t>target_protein_lincs_id</t>
+    <t>target_protein_center_ids</t>
   </si>
   <si>
     <t>AR_Non-Protein_Target</t>
@@ -123,7 +131,7 @@
     <t>natural</t>
   </si>
   <si>
-    <t>HMSL201294</t>
+    <t>HMSL201294; HMSL201295</t>
   </si>
   <si>
     <t>Homo sapiens</t>
@@ -303,6 +311,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -324,6 +333,7 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -331,6 +341,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -338,17 +349,20 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -478,26 +492,26 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.8520408163265"/>
-    <col collapsed="false" hidden="false" max="21" min="10" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.5765306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="794" min="27" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="795" style="0" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="794" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="795" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,7 +527,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="4"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -532,501 +548,501 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" s="9" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="9" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="I2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="J2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V3" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y3" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W4" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y4" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y5" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V6" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W6" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y6" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="V7" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W7" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y7" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V8" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W8" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X8" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y8" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E9" s="12"/>
       <c r="G9" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="S9" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V9" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W9" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X9" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y9" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add long alt-name example
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
   <si>
     <t>not used at this time (but still required in this sheet)</t>
   </si>
@@ -122,7 +122,7 @@
     <t>p-H31 S10</t>
   </si>
   <si>
-    <t>Phospho-Histone H3 (Ser10) (D2C8) XP® Rabbit mAb (Alexa Fluor® 555 Conjugate)</t>
+    <t>ERK-1 (pT202; pY204); ERK1 (pT202); ERK-2 (pT185; pY187); ERK2 (pT185) / AlexaFluor488</t>
   </si>
   <si>
     <t>HMSL80001</t>
@@ -179,7 +179,7 @@
     <t>CDN1A</t>
   </si>
   <si>
-    <t>p21 Waf1/Cip1 (12D1) Rabbit mAb (Alexa Fluor® 647 Conjugate)</t>
+    <t>ERK-2 (pT202; pY204); ERK3 (pT202); ERK-4 (pT185; pY187); ERK5 (pT185) / AlexaFluor488</t>
   </si>
   <si>
     <t>HMSL80002</t>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>D3B5</t>
-  </si>
-  <si>
-    <t>not available</t>
   </si>
   <si>
     <t>HMSL201296</t>
@@ -347,7 +344,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -404,11 +401,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -454,7 +446,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -512,10 +504,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,29 +539,28 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.4744897959184"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="15" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="796" min="29" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="797" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="15" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="797" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,20 +743,20 @@
       <c r="V3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA3" s="15" t="s">
+      <c r="Y3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
         <v>50</v>
       </c>
@@ -798,7 +785,7 @@
       <c r="L4" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="15" t="s">
         <v>57</v>
       </c>
       <c r="N4" s="12" t="s">
@@ -822,21 +809,21 @@
       <c r="U4" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="X4" s="15" t="s">
+      <c r="X4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA4" s="15" t="s">
+      <c r="Y4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -849,26 +836,24 @@
       <c r="F5" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>64</v>
-      </c>
+      <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="N5" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>42</v>
@@ -886,55 +871,53 @@
         <v>43</v>
       </c>
       <c r="U5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="X5" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y5" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z5" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA5" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>71</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>72</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>64</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
         <v>36</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="N6" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>77</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>42</v>
@@ -954,53 +937,53 @@
       <c r="U6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="15" t="s">
+      <c r="X6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA6" s="15" t="s">
+      <c r="Y6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA6" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="N7" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="O7" s="12" t="s">
         <v>42</v>
@@ -1020,53 +1003,53 @@
       <c r="U7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="X7" s="15" t="s">
+      <c r="X7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z7" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA7" s="15" t="s">
+      <c r="Y7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA7" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="N8" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>95</v>
       </c>
       <c r="O8" s="12" t="s">
         <v>42</v>
@@ -1084,74 +1067,74 @@
         <v>43</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="X8" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="X8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA8" s="15" t="s">
+      <c r="Y8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA8" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="E9" s="13"/>
       <c r="G9" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>36</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="17" t="s">
-        <v>101</v>
+      <c r="N9" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="O9" s="13" t="s">
         <v>42</v>
       </c>
       <c r="P9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q9" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="R9" s="13" t="s">
         <v>45</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U9" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="X9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="X9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y9" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z9" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA9" s="15" t="s">
+      <c r="Y9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA9" s="14" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjust word wrap & max width on antibody.name column
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
   <si>
     <t>not used at this time (but still required in this sheet)</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Is Restricted</t>
   </si>
   <si>
-    <t>p-H31 S10</t>
-  </si>
-  <si>
     <t>ERK-1 (pT202; pY204); ERK1 (pT202); ERK-2 (pT185; pY187); ERK2 (pT185) / AlexaFluor488</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
   </si>
   <si>
     <t>2015-09-16</t>
-  </si>
-  <si>
-    <t>CDN1A</t>
   </si>
   <si>
     <t>ERK-2 (pT202; pY204); ERK3 (pT202); ERK-4 (pT185; pY187); ERK5 (pT185) / AlexaFluor488</t>
@@ -539,7 +533,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3:C4"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -692,450 +686,450 @@
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="N3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="12" t="s">
+      <c r="V3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="X3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="Y3" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z3" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA3" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>52</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="K4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="12" t="s">
+      <c r="M4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="0" t="s">
+      <c r="N4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="O4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="X4" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="0" t="s">
+      <c r="N5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="O5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="X5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z5" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA5" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="0" t="s">
+      <c r="N6" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>76</v>
-      </c>
       <c r="O6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="Q6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="R6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="S6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="S6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="X6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z6" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA6" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="K7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="M7" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="0" t="s">
+      <c r="N7" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="M7" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="O7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="S7" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>88</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="K8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="12" t="s">
+      <c r="M8" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="0" t="s">
+      <c r="N8" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>94</v>
-      </c>
       <c r="O8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="R8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="S8" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X8" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>97</v>
       </c>
       <c r="E9" s="13"/>
       <c r="G9" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q9" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="O9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="R9" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U9" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X9" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments field for reagent and reagent_batch, resolves #469
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
   <si>
     <t>not used at this time (but still required in this sheet)</t>
   </si>
@@ -119,6 +119,9 @@
     <t>Is Restricted</t>
   </si>
   <si>
+    <t>Comments</t>
+  </si>
+  <si>
     <t>ERK-1 (pT202; pY204); ERK1 (pT202); ERK-2 (pT185; pY187); ERK2 (pT185) / AlexaFluor488</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
     <t>2015-09-16</t>
   </si>
   <si>
+    <t>ab test comment 1</t>
+  </si>
+  <si>
     <t>ERK-2 (pT202; pY204); ERK3 (pT202); ERK-4 (pT185; pY187); ERK5 (pT185) / AlexaFluor488</t>
   </si>
   <si>
@@ -200,6 +206,9 @@
     <t>Alexa Fluor 647</t>
   </si>
   <si>
+    <t>ab test comment 2</t>
+  </si>
+  <si>
     <t>KI67</t>
   </si>
   <si>
@@ -227,6 +236,9 @@
     <t>Alexa Fluor 488</t>
   </si>
   <si>
+    <t>ab test comment 3</t>
+  </si>
+  <si>
     <t>p-RB1 S807/S811</t>
   </si>
   <si>
@@ -251,6 +263,9 @@
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic phosphopeptide corresponding to residues surrounding Ser807/811 of human Rb protein. (source: Cell Signaling Technology)</t>
   </si>
   <si>
+    <t>ab test comment 4</t>
+  </si>
+  <si>
     <t>p-RS6 S235/S236</t>
   </si>
   <si>
@@ -278,6 +293,9 @@
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic phosphopeptide corresponding to residues surrounding Ser235 and Ser236 of human ribosomal protein S6. (source: Cell Signaling Technology)</t>
   </si>
   <si>
+    <t>ab test comment 5</t>
+  </si>
+  <si>
     <t>p-RS6 S240/S244</t>
   </si>
   <si>
@@ -303,6 +321,9 @@
   </si>
   <si>
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic phosphopeptide corresponding to residues surrounding Ser240 and Ser244 of human ribosomal protein S6. (source: Cell Signaling Technology)</t>
+  </si>
+  <si>
+    <t>ab test comment 6</t>
   </si>
   <si>
     <t>rabbit IgG(H+L)</t>
@@ -328,6 +349,9 @@
   </si>
   <si>
     <t>polyclonal</t>
+  </si>
+  <si>
+    <t>ab test comment 7</t>
   </si>
 </sst>
 </file>
@@ -440,7 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -487,6 +511,10 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -526,35 +554,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AC2" activeCellId="0" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="23" min="15" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="797" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="23" min="15" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="796" min="29" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="797" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,456 +709,480 @@
       <c r="AB2" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="AC2" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>37</v>
       </c>
+      <c r="K3" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="L3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="M3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="N3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="O3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="P3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="Q3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="12" t="s">
+      <c r="R3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="S3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="V3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="X3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA3" s="14" t="s">
-        <v>48</v>
+      <c r="Y3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="C4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="12" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>37</v>
+      <c r="G4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="12" t="s">
+      <c r="M4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="P4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="Q4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="X4" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y4" s="14" t="s">
+      <c r="R4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="Z4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA4" s="14" t="s">
-        <v>48</v>
+      <c r="Y4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>37</v>
+      <c r="D5" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="P5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="Q5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="X5" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y5" s="14" t="s">
+      <c r="R5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="X5" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="Z5" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA5" s="14" t="s">
-        <v>48</v>
+      <c r="Y5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="A6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA6" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC7" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" s="12" t="s">
+      <c r="X8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="G9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="R6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U6" s="12" t="s">
+      <c r="P9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="R9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y6" s="14" t="s">
+      <c r="S9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="U9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="X9" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y7" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z7" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA7" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="X8" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y8" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z8" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA8" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="G9" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="U9" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="X9" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA9" s="14" t="s">
-        <v>48</v>
+      <c r="Y9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC9" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>